<commit_message>
Error analysis - CAD
</commit_message>
<xml_diff>
--- a/Error Analysis/BERT vs. BERT_Augmented.xlsx
+++ b/Error Analysis/BERT vs. BERT_Augmented.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kalyan\Documents\Anu\W266 - NLP\Final Project\lheart-disease-risk-prediction\Error Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4B387B-3035-4F40-A603-1CC401CAB6B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF34D6D-CFDF-4E8D-BD90-11833EA14EFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" activeTab="1" xr2:uid="{18A11775-EDF5-4E2F-8053-1924F40215E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Diabetes Indicator" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="CM-Other-A1C" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t xml:space="preserve">              pred:A1C  pred:Other  pred:glucose  pred:mention</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>BERT</t>
   </si>
 </sst>
 </file>
@@ -735,15 +738,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B405657-8A02-4D26-801B-CF5AE4246FDC}">
-  <dimension ref="R41"/>
+  <dimension ref="I37:AD41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
-      <selection activeCell="R41" sqref="R41"/>
+      <selection activeCell="AD38" sqref="AD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="41" spans="18:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="9:30" x14ac:dyDescent="0.3">
+      <c r="AD37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="9:30" x14ac:dyDescent="0.3">
+      <c r="I38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="9:30" x14ac:dyDescent="0.3">
       <c r="R41" t="s">
         <v>23</v>
       </c>

</xml_diff>